<commit_message>
Update responder guides and documentation
</commit_message>
<xml_diff>
--- a/oib-responder/docs/OpenInfobutton-Responder-Functional-Tests.xlsx
+++ b/oib-responder/docs/OpenInfobutton-Responder-Functional-Tests.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="0" windowWidth="30960" windowHeight="24600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Infobutton Manager" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -181,9 +181,6 @@
 - informationRecipient = patient</t>
   </si>
   <si>
-    <t>- http://www.healthquality.va.gov/diabetes/DM2010_SUM-v4.pdf</t>
-  </si>
-  <si>
     <t>Index expansion</t>
   </si>
   <si>
@@ -251,6 +248,15 @@
   </si>
   <si>
     <t>http://localhost:8080/openInfobutton/responder?mainSearchCriteria.v.c=579.0&amp;mainSearchCriteria.v.cs=2.16.840.1.113883.6.103&amp;taskContext.c.c=PROBLISTREV&amp;age.v.v=5&amp;age.v.u=a</t>
+  </si>
+  <si>
+    <t>- http://www.healthquality.va.gov/diabetes/Final_DM_Pocket_Card_Aug2010.pdf"
+- http://www.healthquality.va.gov/diabetes/DM2010_SUM-v4.pdf
+- http://www.healthquality.va.gov/guidelines/CD/diabetes/24818_48pgs.pdf
+- http://www.healthquality.va.gov/diabetes/cpgSDMDMPOCKETFinalPRESS022513.pdf</t>
+  </si>
+  <si>
+    <t>- http://www.healthquality.va.gov/guidelines/CD/diabetes/24818_48pgs.pdf</t>
   </si>
 </sst>
 </file>
@@ -339,7 +345,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -365,6 +371,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -863,9 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -911,13 +918,13 @@
         <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="60">
+        <v>52</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="48">
       <c r="A3">
         <v>2</v>
       </c>
@@ -931,7 +938,7 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
         <v>37</v>
@@ -951,10 +958,10 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
+        <v>54</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="60">
@@ -962,16 +969,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -982,39 +989,39 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>47</v>
       </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="60">
+    </row>
+    <row r="7" spans="1:21" ht="48">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>50</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>

</xml_diff>